<commit_message>
Nav Names überarbeitet, unit test hinzugefügt, nicht ausprobiert
</commit_message>
<xml_diff>
--- a/BHH PB2 ChallengeIII.xlsx
+++ b/BHH PB2 ChallengeIII.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Pb2-Challenge-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59C01AC-BC08-4F1D-A106-31BA563B0104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F373A5-F451-4ECB-9B9C-5D7BACB5E9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="4MNDoKFtVknnxwKvXWQCEDzvcrBKboRodw2KTelahdgc4DBCUPsyl6xIKcWbZknZbp2pwmzIHrnJz883NsGFtw==" workbookSaltValue="PJ4h/hW2kqjeFYzVhfUXew==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16395" yWindow="270" windowWidth="11640" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bewertungstabelle" sheetId="4" r:id="rId1"/>
@@ -21,17 +21,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,14 +29,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -62,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Teil 1 Bewertungsbogen</t>
   </si>
@@ -132,9 +121,6 @@
   </si>
   <si>
     <t>Gesamtnote (Teil 1 und Teil 2 anteilig nach Punkten - die Kolleg:innen können die Notenliste der Klasse zur Berechnung nutzen)</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Faktor (2-6)</t>
@@ -812,9 +798,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1094,11 +1080,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="50.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.375" style="2" customWidth="1"/>
@@ -1110,12 +1096,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26.1" customHeight="1">
@@ -1147,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>2</v>
@@ -1177,7 +1163,7 @@
     </row>
     <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="25">
@@ -1203,7 +1189,7 @@
     </row>
     <row r="14" spans="1:4" ht="21.75" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="26"/>
@@ -1221,7 +1207,7 @@
     </row>
     <row r="18" spans="1:7" ht="51.95" customHeight="1">
       <c r="A18" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -1232,10 +1218,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>2</v>
@@ -1246,38 +1232,38 @@
         <v>8</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="13" t="e">
+      <c r="C20" s="16">
+        <v>3</v>
+      </c>
+      <c r="D20" s="13">
         <f>C20*B20</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="13" t="e">
+      <c r="C21" s="16">
+        <v>6</v>
+      </c>
+      <c r="D21" s="13">
         <f t="shared" ref="D21:D23" si="1">C21*B21</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="13" t="e">
+      <c r="C22" s="16">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1">
@@ -1285,63 +1271,63 @@
         <v>10</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="13" t="e">
+      <c r="C23" s="16">
+        <v>5</v>
+      </c>
+      <c r="D23" s="13">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.5" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
-      <c r="D24" s="18" t="e">
+      <c r="D24" s="18">
         <f>SUM(D20:D23)</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.5" thickBot="1">
       <c r="A26" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
-      <c r="D26" s="31" t="e">
+      <c r="D26" s="31">
         <f>SUM(D24,D14)</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="45"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" customHeight="1" thickBot="1">
       <c r="A28" s="43"/>
-      <c r="B28" s="32" t="e">
+      <c r="B28" s="32">
         <f>D26/115*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C28" s="46" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="46" cm="1">
         <f t="array" ref="C28">_xlfn.IFS(B28&gt;='Notenspiegel IHK'!$A$2,'Notenspiegel IHK'!$C$2,B28&gt;='Notenspiegel IHK'!$A$3,'Notenspiegel IHK'!$C$3,B28&gt;='Notenspiegel IHK'!$A$4,'Notenspiegel IHK'!$C$4,B28&gt;='Notenspiegel IHK'!$A$5,'Notenspiegel IHK'!$C$5,B28&gt;='Notenspiegel IHK'!$A$6,'Notenspiegel IHK'!$C$6,B28&gt;='Notenspiegel IHK'!$A$7,'Notenspiegel IHK'!$C$7,B28&gt;='Notenspiegel IHK'!$A$8,'Notenspiegel IHK'!$C$8,B28&gt;='Notenspiegel IHK'!$A$9,'Notenspiegel IHK'!$C$9,B28&gt;='Notenspiegel IHK'!$A$10,'Notenspiegel IHK'!$C$10,B28&gt;='Notenspiegel IHK'!$A$11,'Notenspiegel IHK'!$C$11,B28&gt;='Notenspiegel IHK'!$A$12,'Notenspiegel IHK'!$C$12,B28&gt;='Notenspiegel IHK'!$A$13,'Notenspiegel IHK'!$C$13,B28&gt;='Notenspiegel IHK'!$A$14,'Notenspiegel IHK'!$C$14,B28&gt;='Notenspiegel IHK'!$A$15,'Notenspiegel IHK'!$C$15,B28&gt;='Notenspiegel IHK'!$A$16,'Notenspiegel IHK'!$C$16,B28&gt;='Notenspiegel IHK'!$A$17,'Notenspiegel IHK'!$C$17)</f>
-        <v>#VALUE!</v>
+        <v>6</v>
       </c>
       <c r="D28" s="47"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
@@ -1431,7 +1417,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="50.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="2" customWidth="1"/>
@@ -1442,12 +1428,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26.1" customHeight="1">
@@ -1479,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>1</v>
@@ -1505,7 +1491,7 @@
     </row>
     <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
@@ -1535,7 +1521,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1569,7 +1555,7 @@
     </row>
     <row r="20" spans="1:7" ht="51.95" customHeight="1">
       <c r="A20" s="51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
@@ -1580,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>7</v>
@@ -1621,7 +1607,7 @@
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="5">
         <v>5</v>
@@ -1651,7 +1637,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1670,7 +1656,7 @@
         <v>100</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="38.25">
@@ -1680,7 +1666,7 @@
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
@@ -1768,17 +1754,17 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="11" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1866,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1882,7 +1868,7 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="24"/>
@@ -1890,13 +1876,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>37</v>
-      </c>
       <c r="C1" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1907,7 +1893,7 @@
         <v>0.7</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1929,7 +1915,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1940,7 +1926,7 @@
         <v>1.7</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1962,7 +1948,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1973,7 +1959,7 @@
         <v>2.7</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1995,7 +1981,7 @@
         <v>3.3</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2006,7 +1992,7 @@
         <v>3.7</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2028,7 +2014,7 @@
         <v>4.3</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2039,7 +2025,7 @@
         <v>4.7</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2061,7 +2047,7 @@
         <v>5.3</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6">

</xml_diff>